<commit_message>
Finished code for 453.A4
</commit_message>
<xml_diff>
--- a/453 - Natural Language Processing/453.10 - Final Project/vcs_conversations.xlsx
+++ b/453 - Natural Language Processing/453.10 - Final Project/vcs_conversations.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanhayashi/Desktop/Northwestern/NU_MSDS/453 - Natural Language Processing/453.10 - Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7499E30D-3F25-2D4A-8668-F68151A68D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDAFCF6-50A0-AD40-9E64-1776329A860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{25605FB0-9ECE-9F41-9474-5E92CEDC1185}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{25605FB0-9ECE-9F41-9474-5E92CEDC1185}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Conversations" sheetId="1" r:id="rId1"/>
+    <sheet name="Employee" sheetId="3" r:id="rId2"/>
+    <sheet name="Caller" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,32 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Conversation</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Pharmacy</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Sentiment</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
     <t>Caller: Hello, is this The Very Convenient Store? VCS Employee: Yes, it is. How can I assist you today? Caller: Could you tell me your store hours, please? VCS Employee: Certainly. Our general department is open from 8 AM to 8 PM on weekdays, and from 10 AM to 5 PM on weekends. Caller: Wow! Amazing! Those are much better hours than most convenient sores. What other departments do you have? VCS Employee: We also have a pharmacy and a photo department. Caller: Great! Those are all the departments I need in one place. And what are their hours? VCS Employee: The pharmacy and photo departments are open from 9 AM to 5 PM on weekdays. Caller: Great! Those work very well with my working hours, this store is awesome. VCS Employee: You're welcome! If you have any other questions, feel free to call us during our operating hours. Caller: Will do, thanks. Goodbye! VCS Employee: Goodbye, have a great day!</t>
   </si>
   <si>
@@ -99,6 +80,78 @@
   </si>
   <si>
     <t>Caller: Hi, I'm calling about film development. Can you handle various film sizes? VCS Employee: Absolutely, we develop all types of film, regardless of size. Caller: That's just perfect! What's the cost and how quickly can I get my photos? VCS Employee: Film development starts at $5.99 and we can have it ready in just one day. Caller: Only one day? That’s superbly fast, and the price is just right! Do I need to schedule this? VCS Employee: No need for an appointment, we accept walk-ins for film development. Caller: You’ve made my day! Your service sounds truly phenomenal. I'll bring my film in today. Thanks a bunch! VCS Employee: We’re delighted to help and look forward to seeing you. Thank you for choosing our service!</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, it is. How can I assist you today? VCS Employee: Certainly. Our general department is open from 8 AM to 8 PM on weekdays, and from 10 AM to 5 PM on weekends. VCS Employee: We also have a pharmacy and a photo department. VCS Employee: The pharmacy and photo departments are open from 9 AM to 5 PM on weekdays. VCS Employee: You're welcome! If you have any other questions, feel free to call us during our operating hours. VCS Employee: Goodbye, have a great day!</t>
+  </si>
+  <si>
+    <t>VCS Employee: Absolutely! We have a variety of sections including groceries, electronics, home essentials, beauty products, and more. What are you looking for today? VCS Employee: Yes, we have all of those. We offer a wide range of coffee makers, various yoga mats, and a selection of wireless headphones. VCS Employee: We're open from 8 AM to 8 PM on weekdays, and 10 AM to 5 PM on weekends.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, we have a comprehensive grooming section. What specific product are you looking for? VCS Employee: Absolutely, we have a wide variety of razors. Are you looking for a particular brand? VCS Employee: Yes, we do! We have various models of Gillette razors, including the latest ones. VCS Employee: Our Gillette razors start as low as $5.99. We pride ourselves on offering competitive prices.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, indeed! We have an extensive range of school supplies. This includes backpacks, notebooks, pens, pencils, binders, lunch kits, and even a variety of art supplies. VCS Employee: Certainly! For backpacks, we have brands like PackJourney and ShellHarbor. Our notebooks and binders are from well-known names such as Starry Note and Meedo. And for art supplies, we carry brands like CrayArt, as well as a variety of pens and pencils from brands like WriteWell and MarkerPro. VCS Employee: Our prices are very competitive. For instance, PackJourney backpacks start at just $29.99, and Starry Note notebooks are priced as low as $2.49. VCS Employee: We're excited to help you with your back-to-school shopping. If there's anything else you need, just let us know!</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, it is. How may I assist you? VCS Employee: I'm sorry, but our pharmacy is only open from 9 AM to 5 PM on weekdays. VCS Employee: I understand your frustration, and I apologize for any inconvenience. Our hours are set to align with typical business hours, and unfortunately, we're not open beyond those times. VCS Employee: I truly apologize for the inconvenience this causes. We try our best to serve our customers within the given hours. If there's anything else I can do to help within these constraints, please let me know. VCS Employee: I'm sorry to hear that you're disappointed. We value your feedback and will take it into consideration. If there's anything else we can assist you with, please feel free to call us during our operating hours. VCS Employee: Goodbye, and again, I'm sorry for any inconvenience.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, we do have a pharmacy. How can I assist you today? VCS Employee: Our primary service is prescription refills. Unfortunately, we do not offer flu shots or blood pressure readings. VCS Employee: I apologize for any inconvenience. Our focus is on providing efficient prescription refill services. VCS Employee: I'm sorry we couldn't meet all your needs. If you have any prescriptions to fill, we're here to help.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, we have a pharmacy. What can I do for you? VCS Employee: I’m sorry, but prescriptions can only be filled for the person they are prescribed to, and our process usually takes about 48 hours. VCS Employee: Our pharmacy operates from 9 AM to 5 PM on weekdays only, and we are closed on weekends. VCS Employee: I understand your frustration and I apologize for any inconvenience this may cause.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Let me check that for you. May I have your name, please? ...Thank you. I’m looking it up now... Hmm, I’m having a bit of trouble locating your prescription in our system. VCS Employee: I apologize for this delay. Let me check again... Ah, here it is. It appears your prescription is still in process and not ready for pickup. VCS Employee: I'm deeply sorry for the delay and any stress this has caused. We’re doing our best to expedite the process. VCS Employee: I truly apologize for the inconvenience. We hope to resolve this quickly and regain your trust. Goodbye.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Of course! What would you like to know? VCS Employee: Certainly. Our photo department is open from 9 AM to 5 PM on weekdays. VCS Employee: I'm glad to hear that our hours are convenient for you. Is there anything else you need? VCS Employee: The photo department is closed on weekends, but our general department is open from 10 AM to 5 PM on weekends. VCS Employee: I'm pleased to know that. If there's anything specific you need, we're here to help during our weekday hours. VCS Employee: You're very welcome! We're here to assist whenever you need us. Have a wonderful day! VCS Employee: Goodbye!</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, it is! How can I help you today? VCS Employee: Absolutely, we can print any size, from small wallet photos to large posters. Standard 4x6 prints are just $0.15 each. VCS Employee: Yes, we strive to offer great value. And most orders can be completed in just 15 minutes. VCS Employee: No appointment necessary. We’re ready for walk-ins. VCS Employee: We're thrilled to hear that and can't wait to assist you. See you soon!</t>
+  </si>
+  <si>
+    <t>VCS Employee: Yes, we specialize in passport and ID photos, meeting all required specifications. VCS Employee: No limits at all. We cover all standard sizes and specific requirements. VCS Employee: It's only $12.99 for a set, and we can have them ready in about 15 minutes. VCS Employee: Yes, we do require appointments for these photos to ensure quick service. VCS Employee: You're very welcome! We look forward to seeing you and providing excellent service.</t>
+  </si>
+  <si>
+    <t>VCS Employee: Absolutely, we develop all types of film, regardless of size. VCS Employee: Film development starts at $5.99 and we can have it ready in just one day. VCS Employee: No need for an appointment, we accept walk-ins for film development. VCS Employee: We’re delighted to help and look forward to seeing you. Thank you for choosing our service!</t>
+  </si>
+  <si>
+    <t>Caller: Hello, is this The Very Convenient Store?  Caller: Could you tell me your store hours, please? Caller: Wow! Amazing! Those are much better hours than most convenient sores. What other departments do you have? Caller: Great! Those are all the departments I need in one place. And what are their hours? Caller: Great! Those work very well with my working hours, this store is awesome. Caller: Will do, thanks. Goodbye!</t>
+  </si>
+  <si>
+    <t>Caller: Hi, I was wondering if The Very Convenient Store has a general department and what sections you offer? Caller: That's fantastic! Do you carry coffee makers, yoga mats, and wireless headphones? Caller: Amazing! It sounds like you have everything. What are your store hours? Caller: Perfect! Your store seems to have an incredible selection with convenient hours. I'll be stopping by soon!</t>
+  </si>
+  <si>
+    <t>Caller: Hello, I’m looking for grooming products. Do you have a section for that? Caller: I need razors. Do you carry them? Caller: Yes, do you have Gillette razors? Caller: That’s great! How much do they cost? Caller: Wow, that price is incredible! I'm really impressed. I'll be over to buy some today. Thank you!</t>
+  </si>
+  <si>
+    <t>Caller: Hello, I'm getting ready for back-to-school shopping. Does your general department have all the essentials? Caller: Sounds comprehensive! Could you tell me about the brands you have? Caller: That's a fantastic variety! It's great to have such a diverse range of quality options. How are your prices? Caller: That's excellent! It sounds like you've got both variety and value. I'm looking forward to shopping with you for all our school needs!</t>
+  </si>
+  <si>
+    <t>Caller: Hello, is this The Very Convenient Store's pharmacy? Caller: I need to know your pharmacy hours. Are you open late on weekdays or on weekends? Caller: This is unacceptable! Why aren't you open after 5 PM or on weekends? This is highly inconvenient! Caller: This is ridiculous. It's like you don’t care about people who work regular hours. I can't believe this. Caller: No, there's nothing. It's just disappointing. I expected better from your store. Caller: Fine, whatever. Goodbye.</t>
+  </si>
+  <si>
+    <t>Caller: Hello, does The Very Convenient Store have a pharmacy? Caller: I'm curious about what services you offer at your pharmacy. Do you do more than just fill prescriptions? Caller: That's quite limited. Most pharmacies offer those services. It’s really inconvenient that you don’t. Caller: Well, I was hoping for a more comprehensive service. This is disappointing. Thank you anyway.</t>
+  </si>
+  <si>
+    <t>Caller: Hi, I'm calling to ask if you have a pharmacy department? Caller: I need to urgently refill a prescription for my partner. It’s a crucial medication. Can it be done in 24 hours? Caller: This is a major inconvenience! It’s an important medication, and other pharmacies allow family pickups. Plus, are you even open on weekends? Caller: This is unbelievable. You’re not accommodating at all. I’m extremely disappointed with these limitations.</t>
+  </si>
+  <si>
+    <t>Caller: Hello, I dropped off my prescription three days ago. Is it ready yet? Caller: What do you mean you can’t find it? It's been 72 hours! This is unacceptable! Caller: This is ridiculous! It’s been three days. You’re supposed to be reliable. I depend on this medication! Caller: I’m very upset with this service. I'll have to reconsider using your pharmacy in the future. Goodbye.</t>
+  </si>
+  <si>
+    <t>Caller: Hi, I'm calling to inquire about the photo department at The Very Convenient Store. Are you available to assist? Caller: First, could you tell me your weekday hours for the photo department? Caller: That's wonderful! It's so great to find a photo service that's available throughout the week. I'm really happy about that. Caller: Yes, actually. What about your weekend hours? Caller: Oh, I see. Well, it's still fantastic that you're open all weekdays. It works perfectly for me! Caller: Thank you so much. You've been really helpful and this has made my planning much easier! Caller: Thanks, you too! Goodbye!</t>
+  </si>
+  <si>
+    <t>Caller: Hi, is this the photo department at The Very Convenient Store? Caller: I need some digital photos printed. Can you do a variety of sizes? And what are your prices? Caller: That's amazing! Such variety and incredibly affordable too! Caller: Fifteen minutes? That’s phenomenally fast! Do I need an appointment? Caller: This is fantastic! Your service is not just convenient, it's exceptional. I'll be right over. Thank you so much!</t>
+  </si>
+  <si>
+    <t>Caller: Hello, do you offer passport and ID photo services? Caller: Are there size limitations? Caller: Incredible! How much does it cost and how long does it take? Caller: That's a steal! And the speed is just outstanding! Do I need to book in advance? Caller: Perfect! I'm beyond impressed with your efficiency and pricing. I'll schedule an appointment right away. Thanks a ton!</t>
+  </si>
+  <si>
+    <t>Caller: Hi, I'm calling about film development. Can you handle various film sizes? Caller: That's just perfect! What's the cost and how quickly can I get my photos? Caller: Only one day? That’s superbly fast, and the price is just right! Do I need to schedule this? Caller: You’ve made my day! Your service sounds truly phenomenal. I'll bring my film in today. Thanks a bunch!</t>
   </si>
 </sst>
 </file>
@@ -460,201 +513,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAAC132-EC4A-234E-9D9F-65CF09EAC9F1}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF1EF65-1FE2-804D-A810-BFF944E1F50F}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4CA54C-4356-C247-BC82-BEF5F88DF781}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>